<commit_message>
Änderungen der Pings für Lobby
</commit_message>
<xml_diff>
--- a/PingTypen.xlsx
+++ b/PingTypen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fretan-my.sharepoint.com/personal/lukas_tanneberger_fretan_eu/Documents/Dokumente/QNAP funktioniert noch nicht -(   (Zwischenspeicher)/KeplerWolf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="8_{74B24E6A-D33F-478C-B677-8CB9C27F9CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7E035A0-4632-40B5-8D92-C39C56632D50}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="8_{74B24E6A-D33F-478C-B677-8CB9C27F9CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B545849E-0724-498B-8EA8-97F9929AD3FB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3B92A0E8-0C36-43E9-A0F0-099EAA6A0182}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -131,21 +131,6 @@
     <t>VoteAnswerPing</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Dict mit valid </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>∈ {"True", "False") und error ∈ {"", "doppelt", "late"}</t>
-    </r>
-  </si>
-  <si>
     <t>String Spielername</t>
   </si>
   <si>
@@ -180,6 +165,21 @@
   </si>
   <si>
     <t>Dict mit group : String (Gruppe weche gewonnen hat) und players : List of Dict (für jeden Spieler) {name : String, won : String ("True" oder "False"), role : String (Name der Rolle)}</t>
+  </si>
+  <si>
+    <t>Dict mit data: Repräsentation der Spielerdaten (Objekt der Klasse Player) und players : liste der Spielernamen</t>
+  </si>
+  <si>
+    <t>Dict mit valid ∈ {"True", "False"), error ∈ {"", "doppelt", "late"} und players : Liste der Spieler, welche in der Lobby anwesend sind</t>
+  </si>
+  <si>
+    <t>NewLobbyPing</t>
+  </si>
+  <si>
+    <t>Sendet dem Client eine Liste der in der Lobby anwesenden Spieler</t>
+  </si>
+  <si>
+    <t>Liste der Spielernamen</t>
   </si>
 </sst>
 </file>
@@ -555,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D6D1CC-EB1A-4D69-BF41-0E48944867FD}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,12 +686,12 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -700,15 +700,15 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -717,49 +717,49 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -768,15 +768,15 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -785,27 +785,44 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
         <v>41</v>
       </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E15" t="s">
         <v>42</v>
-      </c>
-      <c r="E14" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LobbyPing implementiert, neue Serverstruktur
</commit_message>
<xml_diff>
--- a/PingTypen.xlsx
+++ b/PingTypen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fretan-my.sharepoint.com/personal/lukas_tanneberger_fretan_eu/Documents/Dokumente/QNAP funktioniert noch nicht -(   (Zwischenspeicher)/KeplerWolf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="8_{74B24E6A-D33F-478C-B677-8CB9C27F9CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42C51269-2BF6-401B-9874-66814BF33FA1}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="8_{74B24E6A-D33F-478C-B677-8CB9C27F9CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFFC4AAB-3251-4F1C-A90C-A3833FC7BAC6}"/>
   <bookViews>
     <workbookView xWindow="-21697" yWindow="1388" windowWidth="21795" windowHeight="12974" xr2:uid="{3B92A0E8-0C36-43E9-A0F0-099EAA6A0182}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Datenstruktur</t>
   </si>
   <si>
-    <t>UserNamePing</t>
-  </si>
-  <si>
     <t>Client</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>String</t>
   </si>
   <si>
-    <t>UserNameValidationPing</t>
-  </si>
-  <si>
     <t>Informiert den Client, ob der Name valide ist, ggf. Fehlermeldung</t>
   </si>
   <si>
@@ -192,6 +186,12 @@
   </si>
   <si>
     <t>Dict Spielername -&gt; Rollenbezeichnung</t>
+  </si>
+  <si>
+    <t>UsernamePing</t>
+  </si>
+  <si>
+    <t>UsernameValidationPing</t>
   </si>
 </sst>
 </file>
@@ -570,7 +570,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,274 +601,274 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
         <v>45</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
         <v>48</v>
       </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>50</v>
-      </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
         <v>29</v>
-      </c>
-      <c r="E13" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
         <v>32</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
         <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
         <v>40</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Voting für Werwölfe senden
</commit_message>
<xml_diff>
--- a/PingTypen.xlsx
+++ b/PingTypen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fretan-my.sharepoint.com/personal/lukas_tanneberger_fretan_eu/Documents/Dokumente/QNAP funktioniert noch nicht -(   (Zwischenspeicher)/KeplerWolf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="158" documentId="8_{74B24E6A-D33F-478C-B677-8CB9C27F9CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B9F2F2B-2431-4C6C-B19B-C19AFED89F48}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="8_{74B24E6A-D33F-478C-B677-8CB9C27F9CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C72603AE-99BA-4D23-A78C-7F5468773238}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3B92A0E8-0C36-43E9-A0F0-099EAA6A0182}"/>
+    <workbookView xWindow="-21697" yWindow="1388" windowWidth="21795" windowHeight="12974" xr2:uid="{3B92A0E8-0C36-43E9-A0F0-099EAA6A0182}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -116,9 +116,6 @@
     <t>Sendet dem Client das Ziel des Votings sowie die zur Wahl stehenden Spieler</t>
   </si>
   <si>
-    <t xml:space="preserve">Dict mit type : {Votetypen} und players : Liste der Spielernamen </t>
-  </si>
-  <si>
     <t>Sendet dem Server den Namen, für den abgestimmt wurde</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>Client möchte Lobby verlassen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dict mit type : {Votetypen}, dummy : {"True", "False"} (ob der Client mitvoten soll) und players : Liste der Spielernamen </t>
   </si>
 </sst>
 </file>
@@ -576,7 +576,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,7 +675,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -704,21 +704,21 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
         <v>52</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>53</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
@@ -726,24 +726,24 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>43</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>44</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -752,15 +752,15 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
@@ -769,10 +769,10 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
         <v>48</v>
-      </c>
-      <c r="E11" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -789,7 +789,7 @@
         <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -806,72 +806,72 @@
         <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>31</v>
-      </c>
-      <c r="E15" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
         <v>33</v>
       </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>34</v>
-      </c>
-      <c r="E16" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
         <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
@@ -879,19 +879,19 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>39</v>
-      </c>
-      <c r="E18" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>